<commit_message>
Enviando o novo arquivo de estrturação em Python do projeto de BI para o github - 29/11/2025
</commit_message>
<xml_diff>
--- a/Segundo_Semestre/Analise_de_Dados_Business_intelligence/projeto_hackaton/eOuve - Limeira.xlsx
+++ b/Segundo_Semestre/Analise_de_Dados_Business_intelligence/projeto_hackaton/eOuve - Limeira.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo\OneDrive\Documentos\Área de Trabalho\Códigos e Projetos\Projetos_ADSN_Einstein\Segundo_Semestre\Analise_de_Dados_Business_intelligence\projeto_hackaton\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F730F9B-1177-4449-948B-BD456DA09B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A1730D-FD3F-46E5-BE1F-F4738C8D0249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{3653C60A-380C-4E55-845F-84658C249B33}"/>
+    <workbookView xWindow="3828" yWindow="492" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{3653C60A-380C-4E55-845F-84658C249B33}"/>
   </bookViews>
   <sheets>
     <sheet name="Secret_categ" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="556">
   <si>
     <r>
       <rPr>
@@ -7016,7 +7016,7 @@
         <rFont val="Segoe UI Semibold"/>
         <family val="2"/>
       </rPr>
-      <t>Em andamento</t>
+      <t>Pendente</t>
     </r>
   </si>
   <si>
@@ -7028,32 +7028,7 @@
         <rFont val="Segoe UI Semibold"/>
         <family val="2"/>
       </rPr>
-      <t>Pendente</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10.5"/>
-        <color indexed="63"/>
-        <rFont val="Segoe UI Semibold"/>
-        <family val="2"/>
-      </rPr>
       <t>Assunto</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10.5"/>
-        <color indexed="63"/>
-        <rFont val="Segoe UI Semibold"/>
-        <family val="2"/>
-      </rPr>
-      <t>Em
-andamento</t>
     </r>
   </si>
   <si>
@@ -7126,6 +7101,9 @@
     <t>Secretaria de Obras e
 Serviços Públicos - BUEIROS
 - LIMPEZA</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
   </si>
 </sst>
 </file>
@@ -7357,9 +7335,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7378,6 +7353,12 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -7390,11 +7371,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9952,18 +9930,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="27" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9999,40 +9977,40 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
+        <v>544</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>546</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>548</v>
       </c>
       <c r="B4" s="6">
         <v>172</v>
@@ -10586,7 +10564,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10603,16 +10581,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" s="27" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10631,11 +10609,11 @@
       <c r="E2" s="26" t="s">
         <v>541</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>545</v>
+      <c r="F2" s="40" t="s">
+        <v>555</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>536</v>
@@ -11119,7 +11097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5ECDAD5-963B-466E-B494-04C4CFFC8DD0}">
   <dimension ref="A1:K152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -11139,23 +11117,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="27" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>528</v>
@@ -11218,8 +11196,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>547</v>
+      <c r="A4" s="29" t="s">
+        <v>545</v>
       </c>
       <c r="B4" s="6">
         <v>172</v>
@@ -11442,8 +11420,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
-        <v>551</v>
+      <c r="A11" s="29" t="s">
+        <v>549</v>
       </c>
       <c r="B11" s="6">
         <v>0</v>
@@ -12754,8 +12732,8 @@
       </c>
     </row>
     <row r="52" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="30" t="s">
-        <v>555</v>
+      <c r="A52" s="29" t="s">
+        <v>553</v>
       </c>
       <c r="B52" s="6">
         <v>1</v>
@@ -12818,8 +12796,8 @@
       </c>
     </row>
     <row r="54" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="30" t="s">
-        <v>556</v>
+      <c r="A54" s="29" t="s">
+        <v>554</v>
       </c>
       <c r="B54" s="6">
         <v>0</v>
@@ -13362,8 +13340,8 @@
       </c>
     </row>
     <row r="71" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="30" t="s">
-        <v>554</v>
+      <c r="A71" s="29" t="s">
+        <v>552</v>
       </c>
       <c r="B71" s="6">
         <v>0</v>
@@ -13650,8 +13628,8 @@
       </c>
     </row>
     <row r="80" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="30" t="s">
-        <v>552</v>
+      <c r="A80" s="29" t="s">
+        <v>550</v>
       </c>
       <c r="B80" s="6">
         <v>1</v>
@@ -13970,8 +13948,8 @@
       </c>
     </row>
     <row r="90" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="40" t="s">
-        <v>553</v>
+      <c r="A90" s="35" t="s">
+        <v>551</v>
       </c>
       <c r="B90" s="6">
         <v>36</v>
@@ -14258,8 +14236,8 @@
       </c>
     </row>
     <row r="99" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="32" t="s">
-        <v>550</v>
+      <c r="A99" s="31" t="s">
+        <v>548</v>
       </c>
       <c r="B99" s="13">
         <v>1401</v>
@@ -14802,7 +14780,7 @@
       </c>
     </row>
     <row r="116" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="34" t="s">
+      <c r="A116" s="33" t="s">
         <v>126</v>
       </c>
       <c r="B116" s="6">
@@ -14929,7 +14907,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="120" spans="1:10" s="33" customFormat="1" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" s="32" customFormat="1" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="11" t="s">
         <v>130</v>
       </c>
@@ -15538,8 +15516,8 @@
       </c>
     </row>
     <row r="139" spans="1:10" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="30" t="s">
-        <v>549</v>
+      <c r="A139" s="29" t="s">
+        <v>547</v>
       </c>
       <c r="B139" s="6">
         <v>0</v>
@@ -15809,8 +15787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CBF574-3F75-44EB-83F3-BF1D91EBCD04}">
   <dimension ref="A1:J153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -15826,21 +15804,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" s="27" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>538</v>
@@ -15854,11 +15832,11 @@
       <c r="E2" s="26" t="s">
         <v>541</v>
       </c>
-      <c r="F2" s="28" t="s">
-        <v>545</v>
+      <c r="F2" s="40" t="s">
+        <v>555</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>536</v>
@@ -18489,7 +18467,7 @@
       <c r="H103" s="6">
         <v>53</v>
       </c>
-      <c r="J103" s="39">
+      <c r="J103" s="34">
         <f>SUM(B103:B122)</f>
         <v>62</v>
       </c>
@@ -18521,7 +18499,7 @@
       </c>
     </row>
     <row r="105" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="31" t="s">
+      <c r="A105" s="30" t="s">
         <v>115</v>
       </c>
       <c r="B105" s="6">
@@ -19630,8 +19608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22ECDC0-5661-407C-B0CB-8C1E8A8CAF07}">
   <dimension ref="A1:K281"/>
   <sheetViews>
-    <sheetView topLeftCell="A226" workbookViewId="0">
-      <selection activeCell="J272" sqref="J272"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -19650,18 +19628,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" s="27" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -28356,8 +28334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67003CB9-88D5-4C2A-AF30-406DE4A72C45}">
   <dimension ref="A1:I272"/>
   <sheetViews>
-    <sheetView topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -28373,16 +28351,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>496</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" s="27" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -28401,11 +28379,11 @@
       <c r="E2" s="26" t="s">
         <v>541</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="40" t="s">
+        <v>555</v>
+      </c>
+      <c r="G2" s="26" t="s">
         <v>542</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>543</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>536</v>
@@ -35461,18 +35439,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>497</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>